<commit_message>
Fix circular reference errors in LOE Excel files
Fixed 46 formulas across 11 LOE files:
- Azure Document Intelligence
- Cisco (5 solutions): network-analytics, hybrid-infrastructure, secure-access, ci-cd-automation, sd-wan-enterprise
- Google (2 solutions): landing-zone, modern-workspace
- Microsoft M365 Deployment
- NVIDIA (2 solutions): dgx-superpod, gpu-compute-cluster

Issues fixed:
- SUM formulas referencing ranges that included the formula cell itself
- Self-referencing formulas (e.g., G26 = $G26 + $G26 + ...)
- Corrected SUM ranges to reference actual data rows
</commit_message>
<xml_diff>
--- a/solutions/cisco/ai/network-analytics/presales/level-of-effort-estimate.xlsx
+++ b/solutions/cisco/ai/network-analytics/presales/level-of-effort-estimate.xlsx
@@ -3091,11 +3091,11 @@
         </is>
       </c>
       <c r="D30" s="49">
-        <f>ROUND(SUM(E17:E43)*$C$30,0)</f>
+        <f>ROUND(SUM(E3:E29)*$C$30,0)</f>
         <v/>
       </c>
       <c r="E30" s="51">
-        <f>ROUND(SUM(E17:E43)*0.25,0)</f>
+        <f>ROUND(SUM(E3:E29)*0.25,0)</f>
         <v/>
       </c>
       <c r="F30" s="50" t="n">
@@ -3134,11 +3134,11 @@
         </is>
       </c>
       <c r="D31" s="46">
-        <f>ROUND(SUM(E17:E43)*0.20,0)</f>
+        <f>ROUND(SUM(E3:E30)*0.20,0)</f>
         <v/>
       </c>
       <c r="E31" s="52">
-        <f>ROUND(SUM(E17:E43)*0.20,0)</f>
+        <f>ROUND(SUM(E3:E30)*0.20,0)</f>
         <v/>
       </c>
       <c r="F31" s="47" t="n">
@@ -3170,7 +3170,7 @@
         </is>
       </c>
       <c r="E32" s="54">
-        <f>SUM(E17:E45)</f>
+        <f>SUM(E3:E31)</f>
         <v/>
       </c>
       <c r="F32" s="54" t="inlineStr">
@@ -3179,7 +3179,7 @@
         </is>
       </c>
       <c r="G32" s="54">
-        <f>TEXT(SUM(G17:G45),"$#,##0")</f>
+        <f>TEXT(SUM(G3:G31),"$#,##0")</f>
         <v/>
       </c>
       <c r="H32" s="53" t="inlineStr"/>

</xml_diff>